<commit_message>
Added: - Function to read and separate information from an excel file created.
</commit_message>
<xml_diff>
--- a/src/main/resources/HorarioTeste.xlsx
+++ b/src/main/resources/HorarioTeste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\IdeaProjects\FinalProject\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4556DD9-F039-4CBC-80B8-294AA0AA348C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BC08B5-F40F-451B-83E2-36742C9BCB67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{67F74767-F303-411E-9436-43AE2F261F26}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Horas</t>
   </si>
@@ -97,7 +97,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,8 +125,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,6 +186,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -237,10 +249,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -252,6 +265,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -270,9 +310,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -285,32 +322,12 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -626,7 +643,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14:E16"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,11 +680,11 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="3"/>
@@ -678,9 +695,9 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="17"/>
+      <c r="D3" s="6"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="18"/>
+      <c r="F3" s="7"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -689,20 +706,22 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="17"/>
+      <c r="D4" s="6"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="18"/>
+      <c r="F4" s="7"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="D5" s="24" t="s">
+        <v>9</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="G5" s="3"/>
     </row>
@@ -710,9 +729,9 @@
       <c r="A6" s="2">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B6" s="20"/>
+      <c r="B6" s="9"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="D6" s="24"/>
       <c r="E6" s="1"/>
       <c r="G6" s="3"/>
     </row>
@@ -720,9 +739,9 @@
       <c r="A7" s="2">
         <v>0.4375</v>
       </c>
-      <c r="B7" s="20"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="D7" s="24"/>
       <c r="E7" s="1"/>
       <c r="G7" s="3"/>
     </row>
@@ -730,15 +749,15 @@
       <c r="A8" s="2">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="22" t="s">
+      <c r="D8" s="24"/>
+      <c r="E8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="13" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="3"/>
@@ -747,35 +766,35 @@
       <c r="A9" s="2">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B9" s="20"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="11"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="13"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>0.5</v>
       </c>
-      <c r="B10" s="21"/>
+      <c r="B10" s="10"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="11"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="13"/>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="13" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="1"/>
@@ -784,39 +803,39 @@
       <c r="A12" s="2">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B12" s="9"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="11"/>
+      <c r="F12" s="13"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>0.5625</v>
       </c>
-      <c r="B13" s="10"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="11"/>
+      <c r="F13" s="13"/>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="22" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="16" t="s">
         <v>18</v>
       </c>
       <c r="G14" s="1"/>
@@ -825,22 +844,22 @@
       <c r="A15" s="2">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="14"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="22"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="15"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="23"/>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>0.625</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="14"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="22"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="15"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="23"/>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -849,7 +868,7 @@
       </c>
       <c r="B17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="14" t="s">
         <v>16</v>
       </c>
       <c r="F17" s="1"/>
@@ -861,7 +880,7 @@
       </c>
       <c r="B18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="5"/>
+      <c r="E18" s="14"/>
       <c r="F18" s="1"/>
       <c r="G18" s="4"/>
     </row>
@@ -871,7 +890,7 @@
       </c>
       <c r="B19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="5"/>
+      <c r="E19" s="14"/>
       <c r="F19" s="1"/>
       <c r="G19" s="4"/>
     </row>
@@ -879,10 +898,10 @@
       <c r="A20" s="2">
         <v>0.70833333333333404</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="16" t="s">
         <v>17</v>
       </c>
       <c r="D20" s="1"/>
@@ -894,8 +913,8 @@
       <c r="A21" s="2">
         <v>0.72916666666666696</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="16"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -905,8 +924,8 @@
       <c r="A22" s="2">
         <v>0.75</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="7"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="16"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -918,13 +937,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="F8:F10"/>
+  <mergeCells count="16">
     <mergeCell ref="E17:E19"/>
     <mergeCell ref="B20:B22"/>
     <mergeCell ref="C20:C22"/>
@@ -934,6 +947,13 @@
     <mergeCell ref="C14:C16"/>
     <mergeCell ref="E14:E16"/>
     <mergeCell ref="F14:F16"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="D5:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>